<commit_message>
Updated wild vs. captive muc SIMPER; added core OTUs for con + muc
</commit_message>
<xml_diff>
--- a/WildCaptive/Mucosa/wild.captive.muc_krusk_simper.xlsx
+++ b/WildCaptive/Mucosa/wild.captive.muc_krusk_simper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ecf4928fe261446/Documents/GitHub/Cecum_Microbes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{2B5D70A5-E612-4A9B-8A12-ECED2A2D931F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{8CC2653C-2427-4BF8-9FCF-E063D2CE6591}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
@@ -604,8 +604,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -964,21 +964,21 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="A2:J6"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="90.5703125" customWidth="1"/>
+    <col min="6" max="6" width="89.85546875" customWidth="1"/>
     <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1014,162 +1014,162 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>1.5470800640445001E-2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="2">
         <v>2.18143181854317E-3</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="2">
         <v>2.61771818225181E-2</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="2">
         <v>2.54743448955627E-2</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="2">
         <v>2.0966131558861401E-2</v>
       </c>
-      <c r="I2" s="1">
+      <c r="I2" s="2">
         <v>0</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <v>1.8807167061594299E-2</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="2">
         <v>8.1509715935027E-3</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="2">
         <v>3.26038863740108E-2</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="2">
         <v>7.3658453895498197E-4</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="2">
         <v>9.9794822302615204E-4</v>
       </c>
-      <c r="I3" s="1">
+      <c r="I3" s="2">
         <v>3.1704617245873402E-2</v>
       </c>
-      <c r="J3" s="1">
+      <c r="J3" s="2">
         <v>2.7997114788579601E-2</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="2">
         <v>1.2877626036963999E-2</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="2">
         <v>6.7687411469154902E-3</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="2">
         <v>3.26038863740108E-2</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="2">
         <v>2.14946167341977E-2</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="2">
         <v>2.1993798539443301E-2</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="2">
         <v>2.9021401931311801E-4</v>
       </c>
-      <c r="J4" s="1">
+      <c r="J4" s="2">
         <v>4.7130770823126201E-4</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5">
         <v>1.4902044045217E-2</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5">
         <v>2.8609796356605599E-2</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5">
         <v>8.5829389069816894E-2</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5">
         <v>2.4544373980469599E-2</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5">
         <v>3.1760570759973697E-2</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="1">
         <v>1.30965477500131E-5</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="1">
         <v>3.4650208380017203E-5</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6">
         <v>3.5836038302020597E-2</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6">
         <v>3.59082818150376E-2</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6">
         <v>8.6179876356090201E-2</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6">
         <v>1.0236623663217499E-3</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6">
         <v>1.9849765774661598E-3</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6">
         <v>5.9739096601515003E-2</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6">
         <v>4.3063356043485601E-2</v>
       </c>
     </row>

</xml_diff>